<commit_message>
Updated input data with C_to_T_matching
</commit_message>
<xml_diff>
--- a/Time_series_inputs.xlsx
+++ b/Time_series_inputs.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Loads_solar" sheetId="1" r:id="rId1"/>
     <sheet name="Number_of_days" sheetId="2" r:id="rId2"/>
+    <sheet name="C_to_T_matching" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -6421,7 +6422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6550,4 +6551,2939 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B365"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B365"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>96</v>
+      </c>
+      <c r="B96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>97</v>
+      </c>
+      <c r="B97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>98</v>
+      </c>
+      <c r="B98">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>100</v>
+      </c>
+      <c r="B100">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>101</v>
+      </c>
+      <c r="B101">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>102</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>103</v>
+      </c>
+      <c r="B103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>104</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>105</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>106</v>
+      </c>
+      <c r="B106">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>107</v>
+      </c>
+      <c r="B107">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>108</v>
+      </c>
+      <c r="B108">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>109</v>
+      </c>
+      <c r="B109">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>110</v>
+      </c>
+      <c r="B110">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>111</v>
+      </c>
+      <c r="B111">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>112</v>
+      </c>
+      <c r="B112">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>113</v>
+      </c>
+      <c r="B113">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>114</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>115</v>
+      </c>
+      <c r="B115">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>116</v>
+      </c>
+      <c r="B116">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>117</v>
+      </c>
+      <c r="B117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>118</v>
+      </c>
+      <c r="B118">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>119</v>
+      </c>
+      <c r="B119">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>120</v>
+      </c>
+      <c r="B120">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>121</v>
+      </c>
+      <c r="B121">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>122</v>
+      </c>
+      <c r="B122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>123</v>
+      </c>
+      <c r="B123">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>124</v>
+      </c>
+      <c r="B124">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>125</v>
+      </c>
+      <c r="B125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>126</v>
+      </c>
+      <c r="B126">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>127</v>
+      </c>
+      <c r="B127">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>128</v>
+      </c>
+      <c r="B128">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>129</v>
+      </c>
+      <c r="B129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>130</v>
+      </c>
+      <c r="B130">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>131</v>
+      </c>
+      <c r="B131">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>132</v>
+      </c>
+      <c r="B132">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>133</v>
+      </c>
+      <c r="B133">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>134</v>
+      </c>
+      <c r="B134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>135</v>
+      </c>
+      <c r="B135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>136</v>
+      </c>
+      <c r="B136">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>137</v>
+      </c>
+      <c r="B137">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>138</v>
+      </c>
+      <c r="B138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>139</v>
+      </c>
+      <c r="B139">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>140</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>141</v>
+      </c>
+      <c r="B141">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>142</v>
+      </c>
+      <c r="B142">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>143</v>
+      </c>
+      <c r="B143">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>145</v>
+      </c>
+      <c r="B145">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>146</v>
+      </c>
+      <c r="B146">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>147</v>
+      </c>
+      <c r="B147">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>148</v>
+      </c>
+      <c r="B148">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>149</v>
+      </c>
+      <c r="B149">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>150</v>
+      </c>
+      <c r="B150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>151</v>
+      </c>
+      <c r="B151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>152</v>
+      </c>
+      <c r="B152">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>153</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>154</v>
+      </c>
+      <c r="B154">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>155</v>
+      </c>
+      <c r="B155">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>156</v>
+      </c>
+      <c r="B156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>157</v>
+      </c>
+      <c r="B157">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>158</v>
+      </c>
+      <c r="B158">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>159</v>
+      </c>
+      <c r="B159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>160</v>
+      </c>
+      <c r="B160">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>161</v>
+      </c>
+      <c r="B161">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>162</v>
+      </c>
+      <c r="B162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>163</v>
+      </c>
+      <c r="B163">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>164</v>
+      </c>
+      <c r="B164">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>165</v>
+      </c>
+      <c r="B165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>166</v>
+      </c>
+      <c r="B166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>167</v>
+      </c>
+      <c r="B167">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>168</v>
+      </c>
+      <c r="B168">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>169</v>
+      </c>
+      <c r="B169">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>170</v>
+      </c>
+      <c r="B170">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>171</v>
+      </c>
+      <c r="B171">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>172</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>173</v>
+      </c>
+      <c r="B173">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>174</v>
+      </c>
+      <c r="B174">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>175</v>
+      </c>
+      <c r="B175">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>176</v>
+      </c>
+      <c r="B176">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>177</v>
+      </c>
+      <c r="B177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>178</v>
+      </c>
+      <c r="B178">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>179</v>
+      </c>
+      <c r="B179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>180</v>
+      </c>
+      <c r="B180">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>181</v>
+      </c>
+      <c r="B181">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>182</v>
+      </c>
+      <c r="B182">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>183</v>
+      </c>
+      <c r="B183">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>184</v>
+      </c>
+      <c r="B184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>185</v>
+      </c>
+      <c r="B185">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>186</v>
+      </c>
+      <c r="B186">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>187</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>188</v>
+      </c>
+      <c r="B188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>189</v>
+      </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>190</v>
+      </c>
+      <c r="B190">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>191</v>
+      </c>
+      <c r="B191">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>192</v>
+      </c>
+      <c r="B192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>193</v>
+      </c>
+      <c r="B193">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>194</v>
+      </c>
+      <c r="B194">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>195</v>
+      </c>
+      <c r="B195">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>196</v>
+      </c>
+      <c r="B196">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>197</v>
+      </c>
+      <c r="B197">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>198</v>
+      </c>
+      <c r="B198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>199</v>
+      </c>
+      <c r="B199">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>200</v>
+      </c>
+      <c r="B200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>201</v>
+      </c>
+      <c r="B201">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>202</v>
+      </c>
+      <c r="B202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>203</v>
+      </c>
+      <c r="B203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>204</v>
+      </c>
+      <c r="B204">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>205</v>
+      </c>
+      <c r="B205">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>206</v>
+      </c>
+      <c r="B206">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>207</v>
+      </c>
+      <c r="B207">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>208</v>
+      </c>
+      <c r="B208">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>209</v>
+      </c>
+      <c r="B209">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>210</v>
+      </c>
+      <c r="B210">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>211</v>
+      </c>
+      <c r="B211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>212</v>
+      </c>
+      <c r="B212">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>213</v>
+      </c>
+      <c r="B213">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>214</v>
+      </c>
+      <c r="B214">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>215</v>
+      </c>
+      <c r="B215">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>216</v>
+      </c>
+      <c r="B216">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>217</v>
+      </c>
+      <c r="B217">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>218</v>
+      </c>
+      <c r="B218">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>219</v>
+      </c>
+      <c r="B219">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>220</v>
+      </c>
+      <c r="B220">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>221</v>
+      </c>
+      <c r="B221">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>222</v>
+      </c>
+      <c r="B222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>223</v>
+      </c>
+      <c r="B223">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>224</v>
+      </c>
+      <c r="B224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>225</v>
+      </c>
+      <c r="B225">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>226</v>
+      </c>
+      <c r="B226">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>227</v>
+      </c>
+      <c r="B227">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>228</v>
+      </c>
+      <c r="B228">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>229</v>
+      </c>
+      <c r="B229">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>230</v>
+      </c>
+      <c r="B230">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>231</v>
+      </c>
+      <c r="B231">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>232</v>
+      </c>
+      <c r="B232">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>233</v>
+      </c>
+      <c r="B233">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>234</v>
+      </c>
+      <c r="B234">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>235</v>
+      </c>
+      <c r="B235">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>236</v>
+      </c>
+      <c r="B236">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>237</v>
+      </c>
+      <c r="B237">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>238</v>
+      </c>
+      <c r="B238">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>239</v>
+      </c>
+      <c r="B239">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>240</v>
+      </c>
+      <c r="B240">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>241</v>
+      </c>
+      <c r="B241">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>242</v>
+      </c>
+      <c r="B242">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>243</v>
+      </c>
+      <c r="B243">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>244</v>
+      </c>
+      <c r="B244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>245</v>
+      </c>
+      <c r="B245">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>246</v>
+      </c>
+      <c r="B246">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>247</v>
+      </c>
+      <c r="B247">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>248</v>
+      </c>
+      <c r="B248">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>249</v>
+      </c>
+      <c r="B249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>250</v>
+      </c>
+      <c r="B250">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>251</v>
+      </c>
+      <c r="B251">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>252</v>
+      </c>
+      <c r="B252">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>253</v>
+      </c>
+      <c r="B253">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>254</v>
+      </c>
+      <c r="B254">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>255</v>
+      </c>
+      <c r="B255">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>256</v>
+      </c>
+      <c r="B256">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>257</v>
+      </c>
+      <c r="B257">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>258</v>
+      </c>
+      <c r="B258">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>259</v>
+      </c>
+      <c r="B259">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>260</v>
+      </c>
+      <c r="B260">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>261</v>
+      </c>
+      <c r="B261">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>262</v>
+      </c>
+      <c r="B262">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>263</v>
+      </c>
+      <c r="B263">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>264</v>
+      </c>
+      <c r="B264">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>265</v>
+      </c>
+      <c r="B265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>266</v>
+      </c>
+      <c r="B266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>267</v>
+      </c>
+      <c r="B267">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>268</v>
+      </c>
+      <c r="B268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>269</v>
+      </c>
+      <c r="B269">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>270</v>
+      </c>
+      <c r="B270">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>271</v>
+      </c>
+      <c r="B271">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>272</v>
+      </c>
+      <c r="B272">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>273</v>
+      </c>
+      <c r="B273">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>274</v>
+      </c>
+      <c r="B274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>275</v>
+      </c>
+      <c r="B275">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>276</v>
+      </c>
+      <c r="B276">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>277</v>
+      </c>
+      <c r="B277">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>278</v>
+      </c>
+      <c r="B278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>279</v>
+      </c>
+      <c r="B279">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>280</v>
+      </c>
+      <c r="B280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>281</v>
+      </c>
+      <c r="B281">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>282</v>
+      </c>
+      <c r="B282">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>283</v>
+      </c>
+      <c r="B283">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>284</v>
+      </c>
+      <c r="B284">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>285</v>
+      </c>
+      <c r="B285">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>286</v>
+      </c>
+      <c r="B286">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>287</v>
+      </c>
+      <c r="B287">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>288</v>
+      </c>
+      <c r="B288">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>289</v>
+      </c>
+      <c r="B289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>290</v>
+      </c>
+      <c r="B290">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>291</v>
+      </c>
+      <c r="B291">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>292</v>
+      </c>
+      <c r="B292">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>293</v>
+      </c>
+      <c r="B293">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>294</v>
+      </c>
+      <c r="B294">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>295</v>
+      </c>
+      <c r="B295">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>296</v>
+      </c>
+      <c r="B296">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>297</v>
+      </c>
+      <c r="B297">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>298</v>
+      </c>
+      <c r="B298">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>299</v>
+      </c>
+      <c r="B299">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>300</v>
+      </c>
+      <c r="B300">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>301</v>
+      </c>
+      <c r="B301">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>302</v>
+      </c>
+      <c r="B302">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>303</v>
+      </c>
+      <c r="B303">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>304</v>
+      </c>
+      <c r="B304">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>305</v>
+      </c>
+      <c r="B305">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>306</v>
+      </c>
+      <c r="B306">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>307</v>
+      </c>
+      <c r="B307">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>308</v>
+      </c>
+      <c r="B308">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>309</v>
+      </c>
+      <c r="B309">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>310</v>
+      </c>
+      <c r="B310">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>311</v>
+      </c>
+      <c r="B311">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>312</v>
+      </c>
+      <c r="B312">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>313</v>
+      </c>
+      <c r="B313">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>314</v>
+      </c>
+      <c r="B314">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>315</v>
+      </c>
+      <c r="B315">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>316</v>
+      </c>
+      <c r="B316">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>317</v>
+      </c>
+      <c r="B317">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>318</v>
+      </c>
+      <c r="B318">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>319</v>
+      </c>
+      <c r="B319">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>320</v>
+      </c>
+      <c r="B320">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>321</v>
+      </c>
+      <c r="B321">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>322</v>
+      </c>
+      <c r="B322">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>323</v>
+      </c>
+      <c r="B323">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>324</v>
+      </c>
+      <c r="B324">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>325</v>
+      </c>
+      <c r="B325">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>326</v>
+      </c>
+      <c r="B326">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>327</v>
+      </c>
+      <c r="B327">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>328</v>
+      </c>
+      <c r="B328">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>329</v>
+      </c>
+      <c r="B329">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>330</v>
+      </c>
+      <c r="B330">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>331</v>
+      </c>
+      <c r="B331">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>332</v>
+      </c>
+      <c r="B332">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>333</v>
+      </c>
+      <c r="B333">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>334</v>
+      </c>
+      <c r="B334">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>335</v>
+      </c>
+      <c r="B335">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>336</v>
+      </c>
+      <c r="B336">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>337</v>
+      </c>
+      <c r="B337">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>338</v>
+      </c>
+      <c r="B338">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>339</v>
+      </c>
+      <c r="B339">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>340</v>
+      </c>
+      <c r="B340">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>341</v>
+      </c>
+      <c r="B341">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>342</v>
+      </c>
+      <c r="B342">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>343</v>
+      </c>
+      <c r="B343">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>344</v>
+      </c>
+      <c r="B344">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>345</v>
+      </c>
+      <c r="B345">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>346</v>
+      </c>
+      <c r="B346">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>347</v>
+      </c>
+      <c r="B347">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>348</v>
+      </c>
+      <c r="B348">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>349</v>
+      </c>
+      <c r="B349">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>350</v>
+      </c>
+      <c r="B350">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>351</v>
+      </c>
+      <c r="B351">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>352</v>
+      </c>
+      <c r="B352">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>353</v>
+      </c>
+      <c r="B353">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>354</v>
+      </c>
+      <c r="B354">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>355</v>
+      </c>
+      <c r="B355">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>356</v>
+      </c>
+      <c r="B356">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>357</v>
+      </c>
+      <c r="B357">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>358</v>
+      </c>
+      <c r="B358">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>359</v>
+      </c>
+      <c r="B359">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>360</v>
+      </c>
+      <c r="B360">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>361</v>
+      </c>
+      <c r="B361">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>362</v>
+      </c>
+      <c r="B362">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>363</v>
+      </c>
+      <c r="B363">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>364</v>
+      </c>
+      <c r="B364">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>365</v>
+      </c>
+      <c r="B365">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>